<commit_message>
Testdaten angepasst das Fehler bei Datenbankgruppen Bezeichnung
</commit_message>
<xml_diff>
--- a/src/main/resources/base/owfw7/TestPartWithSml.xlsx
+++ b/src/main/resources/base/owfw7/TestPartWithSml.xlsx
@@ -26,9 +26,6 @@
     <t>such</t>
   </si>
   <si>
-    <t>num</t>
-  </si>
-  <si>
     <t>namebspr</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>1TEST7</t>
   </si>
   <si>
-    <t>Teil:Teil</t>
-  </si>
-  <si>
     <t>schr</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Schraube M6 x100</t>
   </si>
   <si>
-    <t>s.qlang</t>
-  </si>
-  <si>
     <t>Schraube M6 x120</t>
   </si>
   <si>
@@ -90,6 +81,15 @@
   </si>
   <si>
     <t>s.qdurch</t>
+  </si>
+  <si>
+    <t>Teil:Artikel</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>S.qlang</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -488,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -499,30 +499,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -533,13 +533,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>120</v>
@@ -550,13 +550,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -567,13 +567,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>100</v>
@@ -584,13 +584,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>120</v>
@@ -601,13 +601,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>40</v>
@@ -618,13 +618,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -635,13 +635,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>60</v>

</xml_diff>

<commit_message>
zwischenstand für Lagergruppeneigenschaften muss noch getestet werden.
</commit_message>
<xml_diff>
--- a/src/main/resources/base/owfw7/TestPartWithSml.xlsx
+++ b/src/main/resources/base/owfw7/TestPartWithSml.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkellermann\Documents\git\importitnew\src\main\resources\base\owfw7\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-465" windowWidth="0" windowHeight="17685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2040" windowHeight="16800"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 

</xml_diff>